<commit_message>
state specific freezing columns
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/BizFinReview.xlsx
+++ b/requirement/src/main/resources/templates/BizFinReview.xlsx
@@ -527,13 +527,16 @@
   <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF1" sqref="AF1:AF1048576"/>
+      <pane xSplit="3" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="32" max="32" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="34" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="18">

</xml_diff>